<commit_message>
V1.0.3 Add a placeholder that makes it possible for players to download this mod from server. Add a property to check magazine condition before firing, default true. Misc changes by VS.
</commit_message>
<xml_diff>
--- a/Chinese.xlsx
+++ b/Chinese.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21368\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SteamLibrary\steamapps\common\Barotrauma\LocalMods\Vanilla Components Expanded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7291947D-4CF4-4CF8-843C-28B91B32263A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD37BC2-0CBB-4422-B81B-7B2ED3720436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>字段名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -196,6 +196,18 @@
   </si>
   <si>
     <t>Microsoft.Xna.Framework.Input.Keys内所有定义的项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杂项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>checkMagCondition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置是否在开火时检查弹匣耐久</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -227,7 +239,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -330,11 +342,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -354,6 +403,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -363,7 +415,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -646,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A11" sqref="A11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -665,30 +723,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -711,7 +769,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
@@ -732,7 +790,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
@@ -751,7 +809,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -774,7 +832,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
@@ -795,7 +853,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
@@ -816,7 +874,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
@@ -837,7 +895,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -858,7 +916,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
@@ -875,6 +933,29 @@
         <v>40</v>
       </c>
       <c r="G10" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="13" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V1.1.0 Updated Refs Refactor over FindProjectile() Add a new way to define projectiles to find Set Runconfig to Forced Updated Docs
</commit_message>
<xml_diff>
--- a/Chinese.xlsx
+++ b/Chinese.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SteamLibrary\steamapps\common\Barotrauma\LocalMods\Vanilla Components Expanded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD37BC2-0CBB-4422-B81B-7B2ED3720436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73CDE34-01AD-443E-8479-F860B01FFDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>字段名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -208,6 +208,34 @@
   </si>
   <si>
     <t>设置是否在开火时检查弹匣耐久</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>switchableSlots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>为一个用逗号分割的int列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可选弹药所在槽位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于列举弹药来源槽位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注释</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定义此参数将自动覆盖switchableProjectiles所定义的内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>旧版</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -239,7 +267,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -317,32 +345,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -377,13 +379,26 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -400,12 +415,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -415,13 +442,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -704,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:G11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -719,37 +743,41 @@
     <col min="5" max="5" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.6640625" style="1"/>
+    <col min="8" max="8" width="49.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="H1" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -764,205 +792,241 @@
       <c r="F2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="1" t="s">
+      <c r="G2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="13"/>
+      <c r="B3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="F4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
-      <c r="B4" s="5" t="s">
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
+      <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C6" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="1" t="s">
+      <c r="F6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G8" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="1" t="s">
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G9" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="1" t="s">
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="4">
+      <c r="E10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="5" t="s">
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="6" t="b">
+      <c r="E11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B12" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="13" t="b">
+      <c r="E12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="10" t="b">
         <v>1</v>
       </c>
+      <c r="H12" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="A2:A5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Upd: Fixed incorrect doc
</commit_message>
<xml_diff>
--- a/Chinese.xlsx
+++ b/Chinese.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SteamLibrary\steamapps\common\Barotrauma\LocalMods\Vanilla Components Expanded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73CDE34-01AD-443E-8479-F860B01FFDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A2AAA7-1DCC-4CC6-A789-19FE8152AB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>字段名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -236,6 +236,14 @@
   </si>
   <si>
     <t>旧版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Auto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>此参数只对Burst开火模式有效</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -398,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -433,19 +441,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -730,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -748,33 +753,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -804,19 +809,19 @@
       <c r="B3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="15" t="s">
+      <c r="F3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H3" s="4" t="s">
@@ -828,19 +833,19 @@
       <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="15">
+      <c r="F4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="1">
         <v>0</v>
       </c>
       <c r="H4" s="4"/>
@@ -869,23 +874,23 @@
       <c r="A6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>40</v>
+      <c r="F6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="H6" s="3"/>
     </row>
@@ -906,7 +911,7 @@
       <c r="F7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H7" s="4"/>
@@ -928,7 +933,7 @@
       <c r="F8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="4"/>
@@ -948,12 +953,14 @@
         <v>40</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="15">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
@@ -972,7 +979,7 @@
       <c r="F10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="1">
         <v>0</v>
       </c>
       <c r="H10" s="4"/>

</xml_diff>

<commit_message>
Upd: Add paras allowing bots use Semi/Burst weapon correctly Updated Docs
</commit_message>
<xml_diff>
--- a/Chinese.xlsx
+++ b/Chinese.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SteamLibrary\steamapps\common\Barotrauma\LocalMods\Vanilla Components Expanded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A2AAA7-1DCC-4CC6-A789-19FE8152AB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C6474B-2C84-4920-98BF-0329121D6DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>字段名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -244,6 +244,21 @@
   </si>
   <si>
     <t>此参数只对Burst开火模式有效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BotReload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">人机 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Semi/Burst模式下机器人开火间隔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>仅对机器人手中的Semi/Burst模式的武器生效</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -406,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -423,34 +438,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -733,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -753,36 +762,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -805,8 +814,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="13" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -829,8 +838,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="13" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -851,8 +860,8 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -871,7 +880,7 @@
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -895,7 +904,7 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
@@ -917,7 +926,7 @@
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
@@ -939,7 +948,7 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
@@ -963,7 +972,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
@@ -985,8 +994,8 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="13" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1007,28 +1016,54 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="10" t="b">
+      <c r="E12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="H12" s="11"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
V1.1.2 Fixed an issue causinhg weapon status indicator showing up even if character was not aiming the weapon Add a parameter allows bots use SRW in semi/burst mode correctly Removed a loooooot of unused usings Convert SRW class into public Updated Docs
</commit_message>
<xml_diff>
--- a/Chinese.xlsx
+++ b/Chinese.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SteamLibrary\steamapps\common\Barotrauma\LocalMods\Vanilla Components Expanded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C6474B-2C84-4920-98BF-0329121D6DF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F11B65-498A-4F9B-90A7-BF1FF216D0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t>字段名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -259,6 +259,10 @@
   </si>
   <si>
     <t>仅对机器人手中的Semi/Burst模式的武器生效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lerp(reload, reload*4, 1-reload)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -421,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -457,9 +461,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -744,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -756,7 +757,7 @@
     <col min="4" max="4" width="44.08203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.25" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="49.25" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.6640625" style="1"/>
   </cols>
@@ -815,7 +816,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -839,7 +840,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -995,7 +996,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1058,8 +1059,8 @@
       <c r="F13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="7">
-        <v>0.1</v>
+      <c r="G13" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>58</v>

</xml_diff>